<commit_message>
DOC - 1/12 meeting agenda 추가
</commit_message>
<xml_diff>
--- a/0_DOC/Plasma_Gen_Project schedule_20180104.xlsx
+++ b/0_DOC/Plasma_Gen_Project schedule_20180104.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="V1.0" sheetId="14" r:id="rId1"/>
     <sheet name="V1.0_대외" sheetId="15" r:id="rId2"/>
+    <sheet name="1차 meeting" sheetId="16" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">V1.0!$A$1:$BT$33</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
   <si>
     <t>▶기능 정리</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -149,10 +150,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Plasma_Gen_Functioin List_20180104.xlsx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>◇PCB발주</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -184,12 +181,71 @@
     <t>Schedule</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Functioin List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇1차 meeting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M/E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H/W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RS-232 CON type 변경 여부
+ - D-Sub 9-pin : PCB size가 커짐
+ - USB Data line : RS-232 통신용 젠더 제작이 필요함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F/W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RS-232 Control를 위한 Command list 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schematic V2.0으로 진행시 M/E part 반영 가능 여부
+ - Volume / Power key / Plasma key / Reset key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M/E 구조에 따른 V2.0 수정 요청 사항 여부
+ - PCB size 및 외곽 모양
+ - 부품 높이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery 형상 및 CON type 협의
+ - Battery size : L x W x H
+ - Battery 용량 : size에 맞춰 결정해야 함
+ - Battery current : 1A 이상
+ - 사용품 사용시 사용품에 맞춰 CON 결정해야 함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>협의 사항</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양산시 필요한 기능
+ - H/W version 관리
+ - D/L나 board test를 위한 Test Pin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +333,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -292,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -791,11 +856,138 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -911,6 +1103,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -941,9 +1136,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1435,8 +1667,8 @@
       <xdr:rowOff>80395</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>173934</xdr:colOff>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>157369</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>80395</xdr:rowOff>
     </xdr:to>
@@ -1448,7 +1680,58 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6264965" y="3998069"/>
-          <a:ext cx="1918252" cy="0"/>
+          <a:ext cx="7467600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>155712</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>100273</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>165652</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>100273</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="직선 화살표 연결선 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9158908" y="3844012"/>
+          <a:ext cx="4581940" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2443,7 +2726,7 @@
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AY22" sqref="AY22"/>
+      <selection pane="topRight" activeCell="AW28" sqref="AW28:AW30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2470,213 +2753,213 @@
     <row r="2" spans="2:195" s="7" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:195" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
-      <c r="C3" s="87">
+      <c r="C3" s="90">
         <v>11</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="89">
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="92">
         <v>12</v>
       </c>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
-      <c r="Q3" s="90"/>
-      <c r="R3" s="90"/>
-      <c r="S3" s="90"/>
-      <c r="T3" s="90"/>
-      <c r="U3" s="90"/>
-      <c r="V3" s="90"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="90"/>
-      <c r="Y3" s="90"/>
-      <c r="Z3" s="90"/>
-      <c r="AA3" s="90"/>
-      <c r="AB3" s="90"/>
-      <c r="AC3" s="90"/>
-      <c r="AD3" s="90"/>
-      <c r="AE3" s="90"/>
-      <c r="AF3" s="90"/>
-      <c r="AG3" s="90"/>
-      <c r="AH3" s="90"/>
-      <c r="AI3" s="90"/>
-      <c r="AJ3" s="90"/>
-      <c r="AK3" s="90"/>
-      <c r="AL3" s="90"/>
-      <c r="AM3" s="90"/>
-      <c r="AN3" s="90"/>
-      <c r="AO3" s="90"/>
-      <c r="AP3" s="90"/>
-      <c r="AQ3" s="90"/>
-      <c r="AR3" s="90"/>
-      <c r="AS3" s="89">
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="93"/>
+      <c r="T3" s="93"/>
+      <c r="U3" s="93"/>
+      <c r="V3" s="93"/>
+      <c r="W3" s="93"/>
+      <c r="X3" s="93"/>
+      <c r="Y3" s="93"/>
+      <c r="Z3" s="93"/>
+      <c r="AA3" s="93"/>
+      <c r="AB3" s="93"/>
+      <c r="AC3" s="93"/>
+      <c r="AD3" s="93"/>
+      <c r="AE3" s="93"/>
+      <c r="AF3" s="93"/>
+      <c r="AG3" s="93"/>
+      <c r="AH3" s="93"/>
+      <c r="AI3" s="93"/>
+      <c r="AJ3" s="93"/>
+      <c r="AK3" s="93"/>
+      <c r="AL3" s="93"/>
+      <c r="AM3" s="93"/>
+      <c r="AN3" s="93"/>
+      <c r="AO3" s="93"/>
+      <c r="AP3" s="93"/>
+      <c r="AQ3" s="93"/>
+      <c r="AR3" s="93"/>
+      <c r="AS3" s="92">
         <v>1</v>
       </c>
-      <c r="AT3" s="90"/>
-      <c r="AU3" s="90"/>
-      <c r="AV3" s="90"/>
-      <c r="AW3" s="90"/>
-      <c r="AX3" s="90"/>
-      <c r="AY3" s="90"/>
-      <c r="AZ3" s="90"/>
-      <c r="BA3" s="90"/>
-      <c r="BB3" s="90"/>
-      <c r="BC3" s="90"/>
-      <c r="BD3" s="90"/>
-      <c r="BE3" s="90"/>
-      <c r="BF3" s="90"/>
-      <c r="BG3" s="90"/>
-      <c r="BH3" s="90"/>
-      <c r="BI3" s="90"/>
-      <c r="BJ3" s="90"/>
-      <c r="BK3" s="90"/>
-      <c r="BL3" s="90"/>
-      <c r="BM3" s="90"/>
-      <c r="BN3" s="90"/>
-      <c r="BO3" s="90"/>
-      <c r="BP3" s="90"/>
-      <c r="BQ3" s="90"/>
-      <c r="BR3" s="90"/>
-      <c r="BS3" s="90"/>
-      <c r="BT3" s="90"/>
-      <c r="BU3" s="90"/>
-      <c r="BV3" s="90"/>
-      <c r="BW3" s="94"/>
-      <c r="BX3" s="90">
+      <c r="AT3" s="93"/>
+      <c r="AU3" s="93"/>
+      <c r="AV3" s="93"/>
+      <c r="AW3" s="93"/>
+      <c r="AX3" s="93"/>
+      <c r="AY3" s="93"/>
+      <c r="AZ3" s="93"/>
+      <c r="BA3" s="93"/>
+      <c r="BB3" s="93"/>
+      <c r="BC3" s="93"/>
+      <c r="BD3" s="93"/>
+      <c r="BE3" s="93"/>
+      <c r="BF3" s="93"/>
+      <c r="BG3" s="93"/>
+      <c r="BH3" s="93"/>
+      <c r="BI3" s="93"/>
+      <c r="BJ3" s="93"/>
+      <c r="BK3" s="93"/>
+      <c r="BL3" s="93"/>
+      <c r="BM3" s="93"/>
+      <c r="BN3" s="93"/>
+      <c r="BO3" s="93"/>
+      <c r="BP3" s="93"/>
+      <c r="BQ3" s="93"/>
+      <c r="BR3" s="93"/>
+      <c r="BS3" s="93"/>
+      <c r="BT3" s="93"/>
+      <c r="BU3" s="93"/>
+      <c r="BV3" s="93"/>
+      <c r="BW3" s="97"/>
+      <c r="BX3" s="93">
         <v>2</v>
       </c>
-      <c r="BY3" s="90"/>
-      <c r="BZ3" s="90"/>
-      <c r="CA3" s="90"/>
-      <c r="CB3" s="90"/>
-      <c r="CC3" s="90"/>
-      <c r="CD3" s="90"/>
-      <c r="CE3" s="90"/>
-      <c r="CF3" s="90"/>
-      <c r="CG3" s="90"/>
-      <c r="CH3" s="90"/>
-      <c r="CI3" s="90"/>
-      <c r="CJ3" s="90"/>
-      <c r="CK3" s="90"/>
-      <c r="CL3" s="90"/>
-      <c r="CM3" s="90"/>
-      <c r="CN3" s="90"/>
-      <c r="CO3" s="90"/>
-      <c r="CP3" s="90"/>
-      <c r="CQ3" s="90"/>
-      <c r="CR3" s="90"/>
-      <c r="CS3" s="90"/>
-      <c r="CT3" s="90"/>
-      <c r="CU3" s="90"/>
-      <c r="CV3" s="90"/>
-      <c r="CW3" s="90"/>
-      <c r="CX3" s="90"/>
-      <c r="CY3" s="90"/>
-      <c r="CZ3" s="89">
+      <c r="BY3" s="93"/>
+      <c r="BZ3" s="93"/>
+      <c r="CA3" s="93"/>
+      <c r="CB3" s="93"/>
+      <c r="CC3" s="93"/>
+      <c r="CD3" s="93"/>
+      <c r="CE3" s="93"/>
+      <c r="CF3" s="93"/>
+      <c r="CG3" s="93"/>
+      <c r="CH3" s="93"/>
+      <c r="CI3" s="93"/>
+      <c r="CJ3" s="93"/>
+      <c r="CK3" s="93"/>
+      <c r="CL3" s="93"/>
+      <c r="CM3" s="93"/>
+      <c r="CN3" s="93"/>
+      <c r="CO3" s="93"/>
+      <c r="CP3" s="93"/>
+      <c r="CQ3" s="93"/>
+      <c r="CR3" s="93"/>
+      <c r="CS3" s="93"/>
+      <c r="CT3" s="93"/>
+      <c r="CU3" s="93"/>
+      <c r="CV3" s="93"/>
+      <c r="CW3" s="93"/>
+      <c r="CX3" s="93"/>
+      <c r="CY3" s="93"/>
+      <c r="CZ3" s="92">
         <v>3</v>
       </c>
-      <c r="DA3" s="90"/>
-      <c r="DB3" s="90"/>
-      <c r="DC3" s="90"/>
-      <c r="DD3" s="90"/>
-      <c r="DE3" s="90"/>
-      <c r="DF3" s="90"/>
-      <c r="DG3" s="90"/>
-      <c r="DH3" s="90"/>
-      <c r="DI3" s="90"/>
-      <c r="DJ3" s="90"/>
-      <c r="DK3" s="90"/>
-      <c r="DL3" s="90"/>
-      <c r="DM3" s="90"/>
-      <c r="DN3" s="90"/>
-      <c r="DO3" s="90"/>
-      <c r="DP3" s="90"/>
-      <c r="DQ3" s="90"/>
-      <c r="DR3" s="90"/>
-      <c r="DS3" s="90"/>
-      <c r="DT3" s="90"/>
-      <c r="DU3" s="90"/>
-      <c r="DV3" s="90"/>
-      <c r="DW3" s="90"/>
-      <c r="DX3" s="90"/>
-      <c r="DY3" s="90"/>
-      <c r="DZ3" s="90"/>
-      <c r="EA3" s="90"/>
-      <c r="EB3" s="90"/>
-      <c r="EC3" s="90"/>
-      <c r="ED3" s="94"/>
-      <c r="EE3" s="95">
+      <c r="DA3" s="93"/>
+      <c r="DB3" s="93"/>
+      <c r="DC3" s="93"/>
+      <c r="DD3" s="93"/>
+      <c r="DE3" s="93"/>
+      <c r="DF3" s="93"/>
+      <c r="DG3" s="93"/>
+      <c r="DH3" s="93"/>
+      <c r="DI3" s="93"/>
+      <c r="DJ3" s="93"/>
+      <c r="DK3" s="93"/>
+      <c r="DL3" s="93"/>
+      <c r="DM3" s="93"/>
+      <c r="DN3" s="93"/>
+      <c r="DO3" s="93"/>
+      <c r="DP3" s="93"/>
+      <c r="DQ3" s="93"/>
+      <c r="DR3" s="93"/>
+      <c r="DS3" s="93"/>
+      <c r="DT3" s="93"/>
+      <c r="DU3" s="93"/>
+      <c r="DV3" s="93"/>
+      <c r="DW3" s="93"/>
+      <c r="DX3" s="93"/>
+      <c r="DY3" s="93"/>
+      <c r="DZ3" s="93"/>
+      <c r="EA3" s="93"/>
+      <c r="EB3" s="93"/>
+      <c r="EC3" s="93"/>
+      <c r="ED3" s="97"/>
+      <c r="EE3" s="98">
         <v>4</v>
       </c>
-      <c r="EF3" s="95"/>
-      <c r="EG3" s="95"/>
-      <c r="EH3" s="95"/>
-      <c r="EI3" s="95"/>
-      <c r="EJ3" s="95"/>
-      <c r="EK3" s="95"/>
-      <c r="EL3" s="95"/>
-      <c r="EM3" s="95"/>
-      <c r="EN3" s="95"/>
-      <c r="EO3" s="95"/>
-      <c r="EP3" s="95"/>
-      <c r="EQ3" s="95"/>
-      <c r="ER3" s="95"/>
-      <c r="ES3" s="95"/>
-      <c r="ET3" s="95"/>
-      <c r="EU3" s="95"/>
-      <c r="EV3" s="95"/>
-      <c r="EW3" s="95"/>
-      <c r="EX3" s="95"/>
-      <c r="EY3" s="95"/>
-      <c r="EZ3" s="95"/>
-      <c r="FA3" s="95"/>
-      <c r="FB3" s="95"/>
-      <c r="FC3" s="95"/>
-      <c r="FD3" s="95"/>
-      <c r="FE3" s="95"/>
-      <c r="FF3" s="95"/>
-      <c r="FG3" s="95"/>
-      <c r="FH3" s="96"/>
-      <c r="FI3" s="89">
+      <c r="EF3" s="98"/>
+      <c r="EG3" s="98"/>
+      <c r="EH3" s="98"/>
+      <c r="EI3" s="98"/>
+      <c r="EJ3" s="98"/>
+      <c r="EK3" s="98"/>
+      <c r="EL3" s="98"/>
+      <c r="EM3" s="98"/>
+      <c r="EN3" s="98"/>
+      <c r="EO3" s="98"/>
+      <c r="EP3" s="98"/>
+      <c r="EQ3" s="98"/>
+      <c r="ER3" s="98"/>
+      <c r="ES3" s="98"/>
+      <c r="ET3" s="98"/>
+      <c r="EU3" s="98"/>
+      <c r="EV3" s="98"/>
+      <c r="EW3" s="98"/>
+      <c r="EX3" s="98"/>
+      <c r="EY3" s="98"/>
+      <c r="EZ3" s="98"/>
+      <c r="FA3" s="98"/>
+      <c r="FB3" s="98"/>
+      <c r="FC3" s="98"/>
+      <c r="FD3" s="98"/>
+      <c r="FE3" s="98"/>
+      <c r="FF3" s="98"/>
+      <c r="FG3" s="98"/>
+      <c r="FH3" s="99"/>
+      <c r="FI3" s="92">
         <v>5</v>
       </c>
-      <c r="FJ3" s="90"/>
-      <c r="FK3" s="90"/>
-      <c r="FL3" s="90"/>
-      <c r="FM3" s="90"/>
-      <c r="FN3" s="90"/>
-      <c r="FO3" s="90"/>
-      <c r="FP3" s="90"/>
-      <c r="FQ3" s="90"/>
-      <c r="FR3" s="90"/>
-      <c r="FS3" s="90"/>
-      <c r="FT3" s="90"/>
-      <c r="FU3" s="90"/>
-      <c r="FV3" s="90"/>
-      <c r="FW3" s="90"/>
-      <c r="FX3" s="90"/>
-      <c r="FY3" s="90"/>
-      <c r="FZ3" s="90"/>
-      <c r="GA3" s="90"/>
-      <c r="GB3" s="90"/>
-      <c r="GC3" s="90"/>
-      <c r="GD3" s="90"/>
-      <c r="GE3" s="90"/>
-      <c r="GF3" s="90"/>
-      <c r="GG3" s="90"/>
-      <c r="GH3" s="90"/>
-      <c r="GI3" s="90"/>
-      <c r="GJ3" s="90"/>
-      <c r="GK3" s="90"/>
-      <c r="GL3" s="90"/>
-      <c r="GM3" s="94"/>
+      <c r="FJ3" s="93"/>
+      <c r="FK3" s="93"/>
+      <c r="FL3" s="93"/>
+      <c r="FM3" s="93"/>
+      <c r="FN3" s="93"/>
+      <c r="FO3" s="93"/>
+      <c r="FP3" s="93"/>
+      <c r="FQ3" s="93"/>
+      <c r="FR3" s="93"/>
+      <c r="FS3" s="93"/>
+      <c r="FT3" s="93"/>
+      <c r="FU3" s="93"/>
+      <c r="FV3" s="93"/>
+      <c r="FW3" s="93"/>
+      <c r="FX3" s="93"/>
+      <c r="FY3" s="93"/>
+      <c r="FZ3" s="93"/>
+      <c r="GA3" s="93"/>
+      <c r="GB3" s="93"/>
+      <c r="GC3" s="93"/>
+      <c r="GD3" s="93"/>
+      <c r="GE3" s="93"/>
+      <c r="GF3" s="93"/>
+      <c r="GG3" s="93"/>
+      <c r="GH3" s="93"/>
+      <c r="GI3" s="93"/>
+      <c r="GJ3" s="93"/>
+      <c r="GK3" s="93"/>
+      <c r="GL3" s="93"/>
+      <c r="GM3" s="97"/>
     </row>
     <row r="4" spans="2:195" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5"/>
@@ -3261,7 +3544,7 @@
       </c>
     </row>
     <row r="5" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="94" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="9"/>
@@ -3463,7 +3746,7 @@
       <c r="GM5" s="11"/>
     </row>
     <row r="6" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B6" s="91"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="20"/>
@@ -3661,7 +3944,7 @@
       <c r="GM6" s="24"/>
     </row>
     <row r="7" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B7" s="91"/>
+      <c r="B7" s="94"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
@@ -3859,7 +4142,7 @@
       <c r="GM7" s="24"/>
     </row>
     <row r="8" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B8" s="91"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="20"/>
@@ -4057,7 +4340,7 @@
       <c r="GM8" s="24"/>
     </row>
     <row r="9" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B9" s="91"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="20"/>
@@ -4255,7 +4538,7 @@
       <c r="GM9" s="24"/>
     </row>
     <row r="10" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B10" s="92"/>
+      <c r="B10" s="95"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="20"/>
@@ -4451,7 +4734,7 @@
       <c r="GM10" s="24"/>
     </row>
     <row r="11" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="96" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="42"/>
@@ -4661,7 +4944,7 @@
       <c r="GM11" s="44"/>
     </row>
     <row r="12" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B12" s="91"/>
+      <c r="B12" s="94"/>
       <c r="C12" s="47"/>
       <c r="D12" s="45"/>
       <c r="E12" s="48"/>
@@ -4861,7 +5144,7 @@
       <c r="GM12" s="49"/>
     </row>
     <row r="13" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B13" s="91"/>
+      <c r="B13" s="94"/>
       <c r="C13" s="56"/>
       <c r="D13" s="57"/>
       <c r="E13" s="59"/>
@@ -5061,7 +5344,7 @@
       <c r="GM13" s="60"/>
     </row>
     <row r="14" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B14" s="91"/>
+      <c r="B14" s="94"/>
       <c r="C14" s="56"/>
       <c r="D14" s="57"/>
       <c r="E14" s="59"/>
@@ -5259,7 +5542,7 @@
       <c r="GM14" s="60"/>
     </row>
     <row r="15" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B15" s="91"/>
+      <c r="B15" s="94"/>
       <c r="C15" s="56"/>
       <c r="D15" s="57"/>
       <c r="E15" s="59"/>
@@ -5457,7 +5740,7 @@
       <c r="GM15" s="60"/>
     </row>
     <row r="16" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B16" s="91"/>
+      <c r="B16" s="94"/>
       <c r="C16" s="56"/>
       <c r="D16" s="57"/>
       <c r="E16" s="59"/>
@@ -5655,7 +5938,7 @@
       <c r="GM16" s="60"/>
     </row>
     <row r="17" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B17" s="91"/>
+      <c r="B17" s="94"/>
       <c r="C17" s="56"/>
       <c r="D17" s="57"/>
       <c r="E17" s="59"/>
@@ -5853,7 +6136,7 @@
       <c r="GM17" s="60"/>
     </row>
     <row r="18" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B18" s="92"/>
+      <c r="B18" s="95"/>
       <c r="C18" s="52"/>
       <c r="D18" s="50"/>
       <c r="E18" s="53"/>
@@ -7882,7 +8165,7 @@
       <c r="AU28" s="20"/>
       <c r="AV28" s="20"/>
       <c r="AW28" s="20" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="AX28" s="13"/>
       <c r="AY28" s="13"/>
@@ -8081,7 +8364,9 @@
       <c r="AT29" s="20"/>
       <c r="AU29" s="20"/>
       <c r="AV29" s="20"/>
-      <c r="AW29" s="20"/>
+      <c r="AW29" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="AX29" s="13"/>
       <c r="AY29" s="13"/>
       <c r="AZ29" s="20"/>
@@ -8279,7 +8564,9 @@
       <c r="AT30" s="6"/>
       <c r="AU30" s="6"/>
       <c r="AV30" s="6"/>
-      <c r="AW30" s="6"/>
+      <c r="AW30" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="AX30" s="13"/>
       <c r="AY30" s="13"/>
       <c r="AZ30" s="6"/>
@@ -8983,9 +9270,9 @@
   </sheetPr>
   <dimension ref="B1:GM49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BE31" sqref="BE31"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y36" sqref="Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -9012,213 +9299,213 @@
     <row r="2" spans="2:195" s="7" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:195" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
-      <c r="C3" s="87">
+      <c r="C3" s="90">
         <v>11</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="89">
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="92">
         <v>12</v>
       </c>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
-      <c r="Q3" s="90"/>
-      <c r="R3" s="90"/>
-      <c r="S3" s="90"/>
-      <c r="T3" s="90"/>
-      <c r="U3" s="90"/>
-      <c r="V3" s="90"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="90"/>
-      <c r="Y3" s="90"/>
-      <c r="Z3" s="90"/>
-      <c r="AA3" s="90"/>
-      <c r="AB3" s="90"/>
-      <c r="AC3" s="90"/>
-      <c r="AD3" s="90"/>
-      <c r="AE3" s="90"/>
-      <c r="AF3" s="90"/>
-      <c r="AG3" s="90"/>
-      <c r="AH3" s="90"/>
-      <c r="AI3" s="90"/>
-      <c r="AJ3" s="90"/>
-      <c r="AK3" s="90"/>
-      <c r="AL3" s="90"/>
-      <c r="AM3" s="90"/>
-      <c r="AN3" s="90"/>
-      <c r="AO3" s="90"/>
-      <c r="AP3" s="90"/>
-      <c r="AQ3" s="90"/>
-      <c r="AR3" s="90"/>
-      <c r="AS3" s="89">
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="93"/>
+      <c r="T3" s="93"/>
+      <c r="U3" s="93"/>
+      <c r="V3" s="93"/>
+      <c r="W3" s="93"/>
+      <c r="X3" s="93"/>
+      <c r="Y3" s="93"/>
+      <c r="Z3" s="93"/>
+      <c r="AA3" s="93"/>
+      <c r="AB3" s="93"/>
+      <c r="AC3" s="93"/>
+      <c r="AD3" s="93"/>
+      <c r="AE3" s="93"/>
+      <c r="AF3" s="93"/>
+      <c r="AG3" s="93"/>
+      <c r="AH3" s="93"/>
+      <c r="AI3" s="93"/>
+      <c r="AJ3" s="93"/>
+      <c r="AK3" s="93"/>
+      <c r="AL3" s="93"/>
+      <c r="AM3" s="93"/>
+      <c r="AN3" s="93"/>
+      <c r="AO3" s="93"/>
+      <c r="AP3" s="93"/>
+      <c r="AQ3" s="93"/>
+      <c r="AR3" s="93"/>
+      <c r="AS3" s="92">
         <v>1</v>
       </c>
-      <c r="AT3" s="90"/>
-      <c r="AU3" s="90"/>
-      <c r="AV3" s="90"/>
-      <c r="AW3" s="90"/>
-      <c r="AX3" s="90"/>
-      <c r="AY3" s="90"/>
-      <c r="AZ3" s="90"/>
-      <c r="BA3" s="90"/>
-      <c r="BB3" s="90"/>
-      <c r="BC3" s="90"/>
-      <c r="BD3" s="90"/>
-      <c r="BE3" s="90"/>
-      <c r="BF3" s="90"/>
-      <c r="BG3" s="90"/>
-      <c r="BH3" s="90"/>
-      <c r="BI3" s="90"/>
-      <c r="BJ3" s="90"/>
-      <c r="BK3" s="90"/>
-      <c r="BL3" s="90"/>
-      <c r="BM3" s="90"/>
-      <c r="BN3" s="90"/>
-      <c r="BO3" s="90"/>
-      <c r="BP3" s="90"/>
-      <c r="BQ3" s="90"/>
-      <c r="BR3" s="90"/>
-      <c r="BS3" s="90"/>
-      <c r="BT3" s="90"/>
-      <c r="BU3" s="90"/>
-      <c r="BV3" s="90"/>
-      <c r="BW3" s="94"/>
-      <c r="BX3" s="90">
+      <c r="AT3" s="93"/>
+      <c r="AU3" s="93"/>
+      <c r="AV3" s="93"/>
+      <c r="AW3" s="93"/>
+      <c r="AX3" s="93"/>
+      <c r="AY3" s="93"/>
+      <c r="AZ3" s="93"/>
+      <c r="BA3" s="93"/>
+      <c r="BB3" s="93"/>
+      <c r="BC3" s="93"/>
+      <c r="BD3" s="93"/>
+      <c r="BE3" s="93"/>
+      <c r="BF3" s="93"/>
+      <c r="BG3" s="93"/>
+      <c r="BH3" s="93"/>
+      <c r="BI3" s="93"/>
+      <c r="BJ3" s="93"/>
+      <c r="BK3" s="93"/>
+      <c r="BL3" s="93"/>
+      <c r="BM3" s="93"/>
+      <c r="BN3" s="93"/>
+      <c r="BO3" s="93"/>
+      <c r="BP3" s="93"/>
+      <c r="BQ3" s="93"/>
+      <c r="BR3" s="93"/>
+      <c r="BS3" s="93"/>
+      <c r="BT3" s="93"/>
+      <c r="BU3" s="93"/>
+      <c r="BV3" s="93"/>
+      <c r="BW3" s="97"/>
+      <c r="BX3" s="93">
         <v>2</v>
       </c>
-      <c r="BY3" s="90"/>
-      <c r="BZ3" s="90"/>
-      <c r="CA3" s="90"/>
-      <c r="CB3" s="90"/>
-      <c r="CC3" s="90"/>
-      <c r="CD3" s="90"/>
-      <c r="CE3" s="90"/>
-      <c r="CF3" s="90"/>
-      <c r="CG3" s="90"/>
-      <c r="CH3" s="90"/>
-      <c r="CI3" s="90"/>
-      <c r="CJ3" s="90"/>
-      <c r="CK3" s="90"/>
-      <c r="CL3" s="90"/>
-      <c r="CM3" s="90"/>
-      <c r="CN3" s="90"/>
-      <c r="CO3" s="90"/>
-      <c r="CP3" s="90"/>
-      <c r="CQ3" s="90"/>
-      <c r="CR3" s="90"/>
-      <c r="CS3" s="90"/>
-      <c r="CT3" s="90"/>
-      <c r="CU3" s="90"/>
-      <c r="CV3" s="90"/>
-      <c r="CW3" s="90"/>
-      <c r="CX3" s="90"/>
-      <c r="CY3" s="90"/>
-      <c r="CZ3" s="89">
+      <c r="BY3" s="93"/>
+      <c r="BZ3" s="93"/>
+      <c r="CA3" s="93"/>
+      <c r="CB3" s="93"/>
+      <c r="CC3" s="93"/>
+      <c r="CD3" s="93"/>
+      <c r="CE3" s="93"/>
+      <c r="CF3" s="93"/>
+      <c r="CG3" s="93"/>
+      <c r="CH3" s="93"/>
+      <c r="CI3" s="93"/>
+      <c r="CJ3" s="93"/>
+      <c r="CK3" s="93"/>
+      <c r="CL3" s="93"/>
+      <c r="CM3" s="93"/>
+      <c r="CN3" s="93"/>
+      <c r="CO3" s="93"/>
+      <c r="CP3" s="93"/>
+      <c r="CQ3" s="93"/>
+      <c r="CR3" s="93"/>
+      <c r="CS3" s="93"/>
+      <c r="CT3" s="93"/>
+      <c r="CU3" s="93"/>
+      <c r="CV3" s="93"/>
+      <c r="CW3" s="93"/>
+      <c r="CX3" s="93"/>
+      <c r="CY3" s="93"/>
+      <c r="CZ3" s="92">
         <v>3</v>
       </c>
-      <c r="DA3" s="90"/>
-      <c r="DB3" s="90"/>
-      <c r="DC3" s="90"/>
-      <c r="DD3" s="90"/>
-      <c r="DE3" s="90"/>
-      <c r="DF3" s="90"/>
-      <c r="DG3" s="90"/>
-      <c r="DH3" s="90"/>
-      <c r="DI3" s="90"/>
-      <c r="DJ3" s="90"/>
-      <c r="DK3" s="90"/>
-      <c r="DL3" s="90"/>
-      <c r="DM3" s="90"/>
-      <c r="DN3" s="90"/>
-      <c r="DO3" s="90"/>
-      <c r="DP3" s="90"/>
-      <c r="DQ3" s="90"/>
-      <c r="DR3" s="90"/>
-      <c r="DS3" s="90"/>
-      <c r="DT3" s="90"/>
-      <c r="DU3" s="90"/>
-      <c r="DV3" s="90"/>
-      <c r="DW3" s="90"/>
-      <c r="DX3" s="90"/>
-      <c r="DY3" s="90"/>
-      <c r="DZ3" s="90"/>
-      <c r="EA3" s="90"/>
-      <c r="EB3" s="90"/>
-      <c r="EC3" s="90"/>
-      <c r="ED3" s="94"/>
-      <c r="EE3" s="95">
+      <c r="DA3" s="93"/>
+      <c r="DB3" s="93"/>
+      <c r="DC3" s="93"/>
+      <c r="DD3" s="93"/>
+      <c r="DE3" s="93"/>
+      <c r="DF3" s="93"/>
+      <c r="DG3" s="93"/>
+      <c r="DH3" s="93"/>
+      <c r="DI3" s="93"/>
+      <c r="DJ3" s="93"/>
+      <c r="DK3" s="93"/>
+      <c r="DL3" s="93"/>
+      <c r="DM3" s="93"/>
+      <c r="DN3" s="93"/>
+      <c r="DO3" s="93"/>
+      <c r="DP3" s="93"/>
+      <c r="DQ3" s="93"/>
+      <c r="DR3" s="93"/>
+      <c r="DS3" s="93"/>
+      <c r="DT3" s="93"/>
+      <c r="DU3" s="93"/>
+      <c r="DV3" s="93"/>
+      <c r="DW3" s="93"/>
+      <c r="DX3" s="93"/>
+      <c r="DY3" s="93"/>
+      <c r="DZ3" s="93"/>
+      <c r="EA3" s="93"/>
+      <c r="EB3" s="93"/>
+      <c r="EC3" s="93"/>
+      <c r="ED3" s="97"/>
+      <c r="EE3" s="98">
         <v>4</v>
       </c>
-      <c r="EF3" s="95"/>
-      <c r="EG3" s="95"/>
-      <c r="EH3" s="95"/>
-      <c r="EI3" s="95"/>
-      <c r="EJ3" s="95"/>
-      <c r="EK3" s="95"/>
-      <c r="EL3" s="95"/>
-      <c r="EM3" s="95"/>
-      <c r="EN3" s="95"/>
-      <c r="EO3" s="95"/>
-      <c r="EP3" s="95"/>
-      <c r="EQ3" s="95"/>
-      <c r="ER3" s="95"/>
-      <c r="ES3" s="95"/>
-      <c r="ET3" s="95"/>
-      <c r="EU3" s="95"/>
-      <c r="EV3" s="95"/>
-      <c r="EW3" s="95"/>
-      <c r="EX3" s="95"/>
-      <c r="EY3" s="95"/>
-      <c r="EZ3" s="95"/>
-      <c r="FA3" s="95"/>
-      <c r="FB3" s="95"/>
-      <c r="FC3" s="95"/>
-      <c r="FD3" s="95"/>
-      <c r="FE3" s="95"/>
-      <c r="FF3" s="95"/>
-      <c r="FG3" s="95"/>
-      <c r="FH3" s="96"/>
-      <c r="FI3" s="89">
+      <c r="EF3" s="98"/>
+      <c r="EG3" s="98"/>
+      <c r="EH3" s="98"/>
+      <c r="EI3" s="98"/>
+      <c r="EJ3" s="98"/>
+      <c r="EK3" s="98"/>
+      <c r="EL3" s="98"/>
+      <c r="EM3" s="98"/>
+      <c r="EN3" s="98"/>
+      <c r="EO3" s="98"/>
+      <c r="EP3" s="98"/>
+      <c r="EQ3" s="98"/>
+      <c r="ER3" s="98"/>
+      <c r="ES3" s="98"/>
+      <c r="ET3" s="98"/>
+      <c r="EU3" s="98"/>
+      <c r="EV3" s="98"/>
+      <c r="EW3" s="98"/>
+      <c r="EX3" s="98"/>
+      <c r="EY3" s="98"/>
+      <c r="EZ3" s="98"/>
+      <c r="FA3" s="98"/>
+      <c r="FB3" s="98"/>
+      <c r="FC3" s="98"/>
+      <c r="FD3" s="98"/>
+      <c r="FE3" s="98"/>
+      <c r="FF3" s="98"/>
+      <c r="FG3" s="98"/>
+      <c r="FH3" s="99"/>
+      <c r="FI3" s="92">
         <v>5</v>
       </c>
-      <c r="FJ3" s="90"/>
-      <c r="FK3" s="90"/>
-      <c r="FL3" s="90"/>
-      <c r="FM3" s="90"/>
-      <c r="FN3" s="90"/>
-      <c r="FO3" s="90"/>
-      <c r="FP3" s="90"/>
-      <c r="FQ3" s="90"/>
-      <c r="FR3" s="90"/>
-      <c r="FS3" s="90"/>
-      <c r="FT3" s="90"/>
-      <c r="FU3" s="90"/>
-      <c r="FV3" s="90"/>
-      <c r="FW3" s="90"/>
-      <c r="FX3" s="90"/>
-      <c r="FY3" s="90"/>
-      <c r="FZ3" s="90"/>
-      <c r="GA3" s="90"/>
-      <c r="GB3" s="90"/>
-      <c r="GC3" s="90"/>
-      <c r="GD3" s="90"/>
-      <c r="GE3" s="90"/>
-      <c r="GF3" s="90"/>
-      <c r="GG3" s="90"/>
-      <c r="GH3" s="90"/>
-      <c r="GI3" s="90"/>
-      <c r="GJ3" s="90"/>
-      <c r="GK3" s="90"/>
-      <c r="GL3" s="90"/>
-      <c r="GM3" s="94"/>
+      <c r="FJ3" s="93"/>
+      <c r="FK3" s="93"/>
+      <c r="FL3" s="93"/>
+      <c r="FM3" s="93"/>
+      <c r="FN3" s="93"/>
+      <c r="FO3" s="93"/>
+      <c r="FP3" s="93"/>
+      <c r="FQ3" s="93"/>
+      <c r="FR3" s="93"/>
+      <c r="FS3" s="93"/>
+      <c r="FT3" s="93"/>
+      <c r="FU3" s="93"/>
+      <c r="FV3" s="93"/>
+      <c r="FW3" s="93"/>
+      <c r="FX3" s="93"/>
+      <c r="FY3" s="93"/>
+      <c r="FZ3" s="93"/>
+      <c r="GA3" s="93"/>
+      <c r="GB3" s="93"/>
+      <c r="GC3" s="93"/>
+      <c r="GD3" s="93"/>
+      <c r="GE3" s="93"/>
+      <c r="GF3" s="93"/>
+      <c r="GG3" s="93"/>
+      <c r="GH3" s="93"/>
+      <c r="GI3" s="93"/>
+      <c r="GJ3" s="93"/>
+      <c r="GK3" s="93"/>
+      <c r="GL3" s="93"/>
+      <c r="GM3" s="97"/>
     </row>
     <row r="4" spans="2:195" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5"/>
@@ -9803,7 +10090,7 @@
       </c>
     </row>
     <row r="5" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="94" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="9"/>
@@ -10005,7 +10292,7 @@
       <c r="GM5" s="11"/>
     </row>
     <row r="6" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B6" s="91"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="20"/>
@@ -10203,7 +10490,7 @@
       <c r="GM6" s="24"/>
     </row>
     <row r="7" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B7" s="91"/>
+      <c r="B7" s="94"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
@@ -10401,7 +10688,7 @@
       <c r="GM7" s="24"/>
     </row>
     <row r="8" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B8" s="91"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="20"/>
@@ -10599,7 +10886,7 @@
       <c r="GM8" s="24"/>
     </row>
     <row r="9" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B9" s="91"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="20"/>
@@ -10797,7 +11084,7 @@
       <c r="GM9" s="24"/>
     </row>
     <row r="10" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B10" s="92"/>
+      <c r="B10" s="95"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="20"/>
@@ -10993,7 +11280,7 @@
       <c r="GM10" s="24"/>
     </row>
     <row r="11" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="96" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="42"/>
@@ -11203,7 +11490,7 @@
       <c r="GM11" s="44"/>
     </row>
     <row r="12" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B12" s="91"/>
+      <c r="B12" s="94"/>
       <c r="C12" s="47"/>
       <c r="D12" s="45"/>
       <c r="E12" s="48"/>
@@ -11403,7 +11690,7 @@
       <c r="GM12" s="49"/>
     </row>
     <row r="13" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B13" s="91"/>
+      <c r="B13" s="94"/>
       <c r="C13" s="56"/>
       <c r="D13" s="57"/>
       <c r="E13" s="59"/>
@@ -11603,7 +11890,7 @@
       <c r="GM13" s="60"/>
     </row>
     <row r="14" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B14" s="91"/>
+      <c r="B14" s="94"/>
       <c r="C14" s="56"/>
       <c r="D14" s="57"/>
       <c r="E14" s="59"/>
@@ -11801,7 +12088,7 @@
       <c r="GM14" s="60"/>
     </row>
     <row r="15" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B15" s="91"/>
+      <c r="B15" s="94"/>
       <c r="C15" s="56"/>
       <c r="D15" s="57"/>
       <c r="E15" s="59"/>
@@ -11999,7 +12286,7 @@
       <c r="GM15" s="60"/>
     </row>
     <row r="16" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B16" s="91"/>
+      <c r="B16" s="94"/>
       <c r="C16" s="56"/>
       <c r="D16" s="57"/>
       <c r="E16" s="59"/>
@@ -12197,7 +12484,7 @@
       <c r="GM16" s="60"/>
     </row>
     <row r="17" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B17" s="91"/>
+      <c r="B17" s="94"/>
       <c r="C17" s="56"/>
       <c r="D17" s="57"/>
       <c r="E17" s="59"/>
@@ -12395,7 +12682,7 @@
       <c r="GM17" s="60"/>
     </row>
     <row r="18" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B18" s="92"/>
+      <c r="B18" s="95"/>
       <c r="C18" s="52"/>
       <c r="D18" s="50"/>
       <c r="E18" s="53"/>
@@ -12591,8 +12878,8 @@
       <c r="GM18" s="54"/>
     </row>
     <row r="19" spans="2:195" x14ac:dyDescent="0.25">
-      <c r="B19" s="93" t="s">
-        <v>34</v>
+      <c r="B19" s="96" t="s">
+        <v>33</v>
       </c>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
@@ -12613,8 +12900,8 @@
       <c r="Q19" s="40"/>
       <c r="R19" s="43"/>
       <c r="S19" s="43"/>
-      <c r="T19" s="98"/>
-      <c r="U19" s="98"/>
+      <c r="T19" s="88"/>
+      <c r="U19" s="88"/>
       <c r="V19" s="41"/>
       <c r="W19" s="41"/>
       <c r="X19" s="39"/>
@@ -12791,7 +13078,7 @@
       <c r="GM19" s="44"/>
     </row>
     <row r="20" spans="2:195" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="91"/>
+      <c r="B20" s="94"/>
       <c r="C20" s="45"/>
       <c r="D20" s="45"/>
       <c r="E20" s="48"/>
@@ -12823,14 +13110,14 @@
       <c r="AC20" s="68"/>
       <c r="AD20" s="46"/>
       <c r="AE20" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AF20" s="48"/>
       <c r="AG20" s="48"/>
       <c r="AH20" s="48"/>
       <c r="AI20" s="48"/>
       <c r="AJ20" s="68" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AK20" s="46"/>
       <c r="AL20" s="46"/>
@@ -12992,7 +13279,7 @@
       <c r="GM20" s="49"/>
     </row>
     <row r="21" spans="2:195" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="91"/>
+      <c r="B21" s="94"/>
       <c r="C21" s="45"/>
       <c r="D21" s="45"/>
       <c r="E21" s="48"/>
@@ -13010,7 +13297,7 @@
       <c r="Q21" s="45"/>
       <c r="R21" s="48"/>
       <c r="S21" s="66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T21" s="48"/>
       <c r="U21" s="48"/>
@@ -13028,13 +13315,13 @@
       <c r="AG21" s="48"/>
       <c r="AH21" s="48"/>
       <c r="AI21" s="66" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AJ21" s="46"/>
       <c r="AK21" s="46"/>
       <c r="AL21" s="46"/>
       <c r="AM21" s="66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AN21" s="48"/>
       <c r="AO21" s="48"/>
@@ -13194,7 +13481,7 @@
       <c r="GM21" s="49"/>
     </row>
     <row r="22" spans="2:195" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="91"/>
+      <c r="B22" s="94"/>
       <c r="C22" s="45"/>
       <c r="D22" s="45"/>
       <c r="E22" s="48"/>
@@ -13231,7 +13518,7 @@
       <c r="AJ22" s="46"/>
       <c r="AK22" s="46"/>
       <c r="AL22" s="46"/>
-      <c r="AM22" s="97" t="s">
+      <c r="AM22" s="87" t="s">
         <v>25</v>
       </c>
       <c r="AN22" s="48"/>
@@ -13392,7 +13679,7 @@
       <c r="GM22" s="49"/>
     </row>
     <row r="23" spans="2:195" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="91"/>
+      <c r="B23" s="94"/>
       <c r="C23" s="45"/>
       <c r="D23" s="45"/>
       <c r="E23" s="48"/>
@@ -13421,7 +13708,7 @@
       <c r="AB23" s="48"/>
       <c r="AC23" s="46"/>
       <c r="AD23" s="46"/>
-      <c r="AE23" s="99" t="s">
+      <c r="AE23" s="89" t="s">
         <v>24</v>
       </c>
       <c r="AF23" s="48"/>
@@ -13590,7 +13877,7 @@
       <c r="GM23" s="49"/>
     </row>
     <row r="24" spans="2:195" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="91"/>
+      <c r="B24" s="94"/>
       <c r="C24" s="45"/>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
@@ -13786,7 +14073,7 @@
       <c r="GM24" s="49"/>
     </row>
     <row r="25" spans="2:195" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="91"/>
+      <c r="B25" s="94"/>
       <c r="C25" s="45"/>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
@@ -13982,7 +14269,7 @@
       <c r="GM25" s="49"/>
     </row>
     <row r="26" spans="2:195" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="92"/>
+      <c r="B26" s="95"/>
       <c r="C26" s="50"/>
       <c r="D26" s="50"/>
       <c r="E26" s="50"/>
@@ -14236,7 +14523,9 @@
       <c r="BA27" s="20"/>
       <c r="BB27" s="4"/>
       <c r="BC27" s="20"/>
-      <c r="BD27" s="20"/>
+      <c r="BD27" s="66" t="s">
+        <v>41</v>
+      </c>
       <c r="BE27" s="13"/>
       <c r="BF27" s="13"/>
       <c r="BG27" s="20"/>
@@ -14428,7 +14717,7 @@
       <c r="AU28" s="20"/>
       <c r="AV28" s="20"/>
       <c r="AW28" s="20" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="AX28" s="13"/>
       <c r="AY28" s="13"/>
@@ -14628,7 +14917,7 @@
       <c r="AU29" s="20"/>
       <c r="AV29" s="20"/>
       <c r="AW29" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AX29" s="13"/>
       <c r="AY29" s="13"/>
@@ -14828,7 +15117,7 @@
       <c r="AU30" s="6"/>
       <c r="AV30" s="6"/>
       <c r="AW30" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AX30" s="13"/>
       <c r="AY30" s="13"/>
@@ -15522,7 +15811,87 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="91" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="92" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="3" max="3" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="100" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="B4" s="101" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="105" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="106"/>
+    </row>
+    <row r="5" spans="2:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="102"/>
+      <c r="C5" s="107" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="108"/>
+    </row>
+    <row r="6" spans="2:4" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="102"/>
+      <c r="C6" s="107" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="108"/>
+    </row>
+    <row r="7" spans="2:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="103" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="107" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="108"/>
+    </row>
+    <row r="8" spans="2:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B8" s="104"/>
+      <c r="C8" s="109" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="110"/>
+    </row>
+    <row r="9" spans="2:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="111" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="112" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="113"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B8"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="99" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>